<commit_message>
Add documentation before adding submodule to another branch
</commit_message>
<xml_diff>
--- a/Documentation/Reports/TimeReport_AspenBoler.xlsx
+++ b/Documentation/Reports/TimeReport_AspenBoler.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\19042\Downloads\HW\CEN3907\plant-partner\Documentation\Reports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC6BAF9B-0BB1-4039-9728-D72B1BB151C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0203A8E2-1D2B-40C1-852D-9EB0CC0FF561}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{605B5A91-C2DF-4ED5-9E2C-366EB894E8F1}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="26">
   <si>
     <t>Name:</t>
   </si>
@@ -108,6 +108,12 @@
   </si>
   <si>
     <t xml:space="preserve">Check-in 3: Met with group &amp; Tyler, discussed things to prepare for alpha build completion and resources to buy </t>
+  </si>
+  <si>
+    <t>Research</t>
+  </si>
+  <si>
+    <t>Began researching ESP32-Wroom and how to develop code; Found IDF with example/interfaces and made into submodule;</t>
   </si>
 </sst>
 </file>
@@ -672,8 +678,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25321167-01B1-413D-AB29-4165F3CF20BA}">
   <dimension ref="A1:F199"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -698,7 +704,7 @@
       </c>
       <c r="E1" s="6">
         <f>SUM(E4:E199)</f>
-        <v>0.48125000000000007</v>
+        <v>2.4305555555555636E-2</v>
       </c>
       <c r="F1" s="15"/>
     </row>
@@ -934,15 +940,23 @@
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A14" s="7"/>
-      <c r="B14" s="8"/>
-      <c r="C14" s="8"/>
+      <c r="A14" s="7">
+        <v>45954</v>
+      </c>
+      <c r="B14" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="C14" s="9">
+        <v>0.45694444444444443</v>
+      </c>
       <c r="D14" s="8"/>
       <c r="E14" s="10">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F14" s="13"/>
+        <v>-0.45694444444444443</v>
+      </c>
+      <c r="F14" s="13" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" s="7"/>

</xml_diff>

<commit_message>
Updated summary of work + removed temporary main
</commit_message>
<xml_diff>
--- a/Documentation/Reports/TimeReport_AspenBoler.xlsx
+++ b/Documentation/Reports/TimeReport_AspenBoler.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\19042\Downloads\HW\CEN3907\plant-partner\Documentation\Reports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0203A8E2-1D2B-40C1-852D-9EB0CC0FF561}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD08986B-FB33-41C8-9AB7-17CDA3F5F053}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{605B5A91-C2DF-4ED5-9E2C-366EB894E8F1}"/>
+    <workbookView xWindow="0" yWindow="1524" windowWidth="17280" windowHeight="9528" xr2:uid="{605B5A91-C2DF-4ED5-9E2C-366EB894E8F1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="27">
   <si>
     <t>Name:</t>
   </si>
@@ -113,7 +113,10 @@
     <t>Research</t>
   </si>
   <si>
-    <t>Began researching ESP32-Wroom and how to develop code; Found IDF with example/interfaces and made into submodule;</t>
+    <t>Began researching ESP32-Wroom and how to develop code; Found IDF with example/interfaces and made into submodule; Used submodule to configure ESP_IDF on Vscode and examine example projects</t>
+  </si>
+  <si>
+    <t>Design Draft/Plans</t>
   </si>
 </sst>
 </file>
@@ -299,7 +302,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -333,6 +336,9 @@
     </xf>
     <xf numFmtId="46" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -678,8 +684,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25321167-01B1-413D-AB29-4165F3CF20BA}">
   <dimension ref="A1:F199"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -734,7 +740,7 @@
         <v>45933</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="C4" s="9">
         <v>0.47013888888888888</v>
@@ -949,7 +955,7 @@
       <c r="C14" s="9">
         <v>0.45694444444444443</v>
       </c>
-      <c r="D14" s="8"/>
+      <c r="D14" s="17"/>
       <c r="E14" s="10">
         <f t="shared" si="0"/>
         <v>-0.45694444444444443</v>

</xml_diff>

<commit_message>
Updated timesheet for beginning of meet up
</commit_message>
<xml_diff>
--- a/Documentation/Reports/TimeReport_AspenBoler.xlsx
+++ b/Documentation/Reports/TimeReport_AspenBoler.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\19042\Downloads\HW\CEN3907\plant-partner\Documentation\Reports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B61EC5B8-15A6-4CE9-989D-91A3443B8074}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B64A090A-700A-492B-B3FE-6EED41F0CD77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="1524" windowWidth="17280" windowHeight="9528" xr2:uid="{605B5A91-C2DF-4ED5-9E2C-366EB894E8F1}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="29">
   <si>
     <t>Name:</t>
   </si>
@@ -118,13 +118,19 @@
   <si>
     <t>Design Draft/Plans</t>
   </si>
+  <si>
+    <t>Pre-Alpha Dev.</t>
+  </si>
+  <si>
+    <t>Flashed onto all three ESP32's, helped members install development on computers, defined structure for Sunday's end</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="[$-409]h:mm\ AM/PM;@"/>
+    <numFmt numFmtId="164" formatCode="[$-409]h:mm\ AM/PM;@"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -341,10 +347,10 @@
     <xf numFmtId="14" fontId="0" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="3" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -690,8 +696,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25321167-01B1-413D-AB29-4165F3CF20BA}">
   <dimension ref="A1:F199"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -716,7 +722,7 @@
       </c>
       <c r="E1" s="6">
         <f>SUM(E4:E199)</f>
-        <v>0.59583333333333344</v>
+        <v>-8.3333333333331927E-3</v>
       </c>
       <c r="F1" s="15"/>
     </row>
@@ -973,15 +979,23 @@
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A15" s="7"/>
-      <c r="B15" s="8"/>
-      <c r="C15" s="17"/>
+      <c r="A15" s="7">
+        <v>45954</v>
+      </c>
+      <c r="B15" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C15" s="17">
+        <v>0.60416666666666663</v>
+      </c>
       <c r="D15" s="17"/>
       <c r="E15" s="10">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F15" s="13"/>
+        <v>-0.60416666666666663</v>
+      </c>
+      <c r="F15" s="13" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" s="7"/>

</xml_diff>